<commit_message>
updated microzed pinout tables with new hdmi carrier connections
</commit_message>
<xml_diff>
--- a/reference/MicroZed JX pinout tables - HDMI test board pins.xlsx
+++ b/reference/MicroZed JX pinout tables - HDMI test board pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Developer\lupa300\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149D3F90-607A-4314-AB3C-11AEBE00701D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9448C9F9-8EEB-49A4-AEA0-FED726276424}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13014" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JX1" sheetId="2" r:id="rId1"/>
@@ -19,17 +19,22 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="197">
   <si>
     <t>JX2
 Pin</t>
@@ -484,73 +489,148 @@
     <t>NetJX1_100</t>
   </si>
   <si>
-    <t>input data2+</t>
-  </si>
-  <si>
-    <t>input data2-</t>
-  </si>
-  <si>
-    <t>input data1+</t>
-  </si>
-  <si>
-    <t>input data1-</t>
-  </si>
-  <si>
-    <t>input data0-</t>
-  </si>
-  <si>
-    <t>input data0+</t>
-  </si>
-  <si>
-    <t>input clock+</t>
-  </si>
-  <si>
-    <t>input clock-</t>
-  </si>
-  <si>
     <t>HDMI BOARD CONNECTION</t>
   </si>
   <si>
-    <t>output data2+</t>
-  </si>
-  <si>
-    <t>output data2-</t>
-  </si>
-  <si>
-    <t>output data1+</t>
-  </si>
-  <si>
-    <t>output data1-</t>
-  </si>
-  <si>
-    <t>output data0+</t>
-  </si>
-  <si>
-    <t>output data0-</t>
-  </si>
-  <si>
-    <t>output clock+</t>
-  </si>
-  <si>
-    <t>output clock-</t>
-  </si>
-  <si>
-    <t>hotplug detect mosfet control</t>
-  </si>
-  <si>
     <t>hdmi in scl</t>
   </si>
   <si>
     <t>hdmi in sda</t>
   </si>
   <si>
-    <t>prog oscillator scl (need internal pullup)</t>
-  </si>
-  <si>
-    <t>prog oscillator sda (need internal pullup)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">programmable osc. Input </t>
+    <t>hdmi out clock+</t>
+  </si>
+  <si>
+    <t>hdmi out clock-</t>
+  </si>
+  <si>
+    <t>hdmi out data0+</t>
+  </si>
+  <si>
+    <t>hdmi out data0-</t>
+  </si>
+  <si>
+    <t>hdmi out data1+</t>
+  </si>
+  <si>
+    <t>hdmi out data2+</t>
+  </si>
+  <si>
+    <t>hdmi out data1-</t>
+  </si>
+  <si>
+    <t>hdmi out data2-</t>
+  </si>
+  <si>
+    <t>lupa spi enable</t>
+  </si>
+  <si>
+    <t>lupa spi clock</t>
+  </si>
+  <si>
+    <t>lupa spi data</t>
+  </si>
+  <si>
+    <t>lupa reset</t>
+  </si>
+  <si>
+    <t>lupa line valid</t>
+  </si>
+  <si>
+    <t>lupa frame valid</t>
+  </si>
+  <si>
+    <t>lupa int time3</t>
+  </si>
+  <si>
+    <t>lupa int time1</t>
+  </si>
+  <si>
+    <t>lupa int time2</t>
+  </si>
+  <si>
+    <t>lupa clock</t>
+  </si>
+  <si>
+    <t>prog osc sda</t>
+  </si>
+  <si>
+    <t>proc osc scl</t>
+  </si>
+  <si>
+    <t>lupa power enable</t>
+  </si>
+  <si>
+    <t>prog osc clock in</t>
+  </si>
+  <si>
+    <t>lupa d9</t>
+  </si>
+  <si>
+    <t>lupa d8</t>
+  </si>
+  <si>
+    <t>lupa d7</t>
+  </si>
+  <si>
+    <t>lupa d6</t>
+  </si>
+  <si>
+    <t>lupa d5</t>
+  </si>
+  <si>
+    <t>lupa d4</t>
+  </si>
+  <si>
+    <t>lupa d3</t>
+  </si>
+  <si>
+    <t>lupa d2</t>
+  </si>
+  <si>
+    <t>lupa d1</t>
+  </si>
+  <si>
+    <t>lupa d0</t>
+  </si>
+  <si>
+    <t>hdmi in clock+</t>
+  </si>
+  <si>
+    <t>hdmi in clock-</t>
+  </si>
+  <si>
+    <t>hdmi in data0+</t>
+  </si>
+  <si>
+    <t>hdmi in data0-</t>
+  </si>
+  <si>
+    <t>hdmi in data1+</t>
+  </si>
+  <si>
+    <t>hdmi in data1-</t>
+  </si>
+  <si>
+    <t>hdmi in data2+</t>
+  </si>
+  <si>
+    <t>hdmi in data2-</t>
+  </si>
+  <si>
+    <t>hdmi hot plug  control, high level pulls hotplug low</t>
+  </si>
+  <si>
+    <t>led1</t>
+  </si>
+  <si>
+    <t>led2</t>
+  </si>
+  <si>
+    <t>led3</t>
+  </si>
+  <si>
+    <t>led4</t>
   </si>
 </sst>
 </file>
@@ -8519,21 +8599,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" customWidth="1"/>
-    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
@@ -8550,10 +8630,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -8573,7 +8653,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -8593,7 +8673,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -8613,7 +8693,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -8633,7 +8713,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -8653,7 +8733,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -8673,7 +8753,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -8693,7 +8773,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -8713,7 +8793,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -8733,7 +8813,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -8753,7 +8833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -8772,8 +8852,11 @@
         <f>+VLOOKUP($C12,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -8792,8 +8875,11 @@
         <f>+VLOOKUP($C13,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -8813,7 +8899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -8832,8 +8918,11 @@
         <f>+VLOOKUP($C15,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -8853,7 +8942,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -8873,7 +8962,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -8893,10 +8982,10 @@
         <v>34</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -8915,8 +9004,11 @@
         <f>+VLOOKUP($C19,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -8936,10 +9028,10 @@
         <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -8959,7 +9051,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -8979,7 +9071,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -8999,7 +9091,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -9018,11 +9110,8 @@
         <f>+VLOOKUP($C24,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -9041,8 +9130,11 @@
         <f>+VLOOKUP($C25,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -9061,11 +9153,8 @@
         <f>+VLOOKUP($C26,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -9084,8 +9173,11 @@
         <f>+VLOOKUP($C27,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -9105,7 +9197,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -9125,7 +9217,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -9144,11 +9236,8 @@
         <f>+VLOOKUP($C30,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -9167,8 +9256,11 @@
         <f>+VLOOKUP($C31,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -9187,11 +9279,8 @@
         <f>+VLOOKUP($C32,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F32" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -9210,8 +9299,11 @@
         <f>+VLOOKUP($C33,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -9231,7 +9323,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -9251,7 +9343,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -9270,11 +9362,8 @@
         <f>+VLOOKUP($C36,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F36" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -9293,8 +9382,11 @@
         <f>+VLOOKUP($C37,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -9313,11 +9405,8 @@
         <f>+VLOOKUP($C38,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -9336,8 +9425,11 @@
         <f>+VLOOKUP($C39,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -9357,7 +9449,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -9377,7 +9469,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -9397,7 +9489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -9416,8 +9508,11 @@
         <f>+VLOOKUP($C43,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -9437,7 +9532,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -9457,7 +9552,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -9477,7 +9572,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -9497,7 +9592,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -9516,11 +9611,8 @@
         <f>+VLOOKUP($C48,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F48" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -9539,8 +9631,11 @@
         <f>+VLOOKUP($C49,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -9559,11 +9654,8 @@
         <f>+VLOOKUP($C50,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F50" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -9582,8 +9674,11 @@
         <f>+VLOOKUP($C51,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -9603,7 +9698,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -9623,7 +9718,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -9642,11 +9737,8 @@
         <f>+VLOOKUP($C54,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F54" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -9665,8 +9757,11 @@
         <f>+VLOOKUP($C55,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -9685,11 +9780,8 @@
         <f>+VLOOKUP($C56,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F56" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -9708,8 +9800,11 @@
         <f>+VLOOKUP($C57,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -9729,7 +9824,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -9749,7 +9844,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -9769,7 +9864,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -9789,7 +9884,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -9808,11 +9903,8 @@
         <f>+VLOOKUP($C62,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F62" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -9831,8 +9923,11 @@
         <f>+VLOOKUP($C63,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -9851,11 +9946,8 @@
         <f>+VLOOKUP($C64,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F64" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -9874,8 +9966,11 @@
         <f>+VLOOKUP($C65,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -9895,7 +9990,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -9915,7 +10010,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -9934,11 +10029,8 @@
         <f>+VLOOKUP($C68,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F68" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -9957,8 +10049,11 @@
         <f>+VLOOKUP($C69,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -9977,9 +10072,6 @@
         <f>+VLOOKUP($C70,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
       </c>
-      <c r="F70" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
@@ -9999,6 +10091,9 @@
       <c r="E71" s="2">
         <f>+VLOOKUP($C71,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>34</v>
+      </c>
+      <c r="F71" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -10611,21 +10706,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.375" customWidth="1"/>
-    <col min="6" max="6" width="32.75" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="40.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10642,10 +10737,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -10665,7 +10760,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -10685,7 +10780,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -10705,7 +10800,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -10725,7 +10820,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -10745,7 +10840,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -10765,7 +10860,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -10785,7 +10880,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -10805,7 +10900,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -10825,7 +10920,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -10845,7 +10940,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -10865,7 +10960,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -10885,7 +10980,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -10905,7 +11000,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -10925,7 +11020,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -10945,7 +11040,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -10965,7 +11060,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -10984,8 +11079,11 @@
         <f>+VLOOKUP($C18,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -11004,11 +11102,8 @@
         <f>+VLOOKUP($C19,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="F19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -11027,8 +11122,11 @@
         <f>+VLOOKUP($C20,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -11048,7 +11146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -11068,7 +11166,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -11088,7 +11186,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -11107,8 +11205,11 @@
         <f>+VLOOKUP($C24,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -11127,11 +11228,8 @@
         <f>+VLOOKUP($C25,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="F25" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -11150,8 +11248,11 @@
         <f>+VLOOKUP($C26,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -11170,11 +11271,8 @@
         <f>+VLOOKUP($C27,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="F27" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -11194,7 +11292,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -11214,7 +11312,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -11233,8 +11331,11 @@
         <f>+VLOOKUP($C30,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -11253,11 +11354,8 @@
         <f>+VLOOKUP($C31,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="F31" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="14.95" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -11276,8 +11374,11 @@
         <f>+VLOOKUP($C32,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -11296,11 +11397,8 @@
         <f>+VLOOKUP($C33,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="F33" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -11320,7 +11418,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -11340,7 +11438,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -11359,8 +11457,11 @@
         <f>+VLOOKUP($C36,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -11380,7 +11481,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -11399,8 +11500,11 @@
         <f>+VLOOKUP($C38,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -11420,7 +11524,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -11440,7 +11544,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -11460,7 +11564,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -11479,8 +11583,11 @@
         <f>+VLOOKUP($C42,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -11500,7 +11607,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -11519,8 +11626,11 @@
         <f>+VLOOKUP($C44,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -11540,7 +11650,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -11560,7 +11670,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -11580,7 +11690,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -11600,7 +11710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -11619,11 +11729,8 @@
         <f>+VLOOKUP($C49,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-      <c r="F49" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -11643,7 +11750,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -11663,7 +11770,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -11683,7 +11790,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -11703,7 +11810,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -11722,8 +11829,11 @@
         <f>+VLOOKUP($C54,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -11742,8 +11852,11 @@
         <f>+VLOOKUP($C55,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -11762,8 +11875,11 @@
         <f>+VLOOKUP($C56,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -11783,7 +11899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -11803,7 +11919,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -11823,7 +11939,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -11843,7 +11959,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -11863,7 +11979,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -11882,8 +11998,11 @@
         <f>+VLOOKUP($C62,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -11903,7 +12022,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -11922,8 +12041,11 @@
         <f>+VLOOKUP($C64,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -11943,7 +12065,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -11963,7 +12085,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -11983,7 +12105,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -12002,8 +12124,11 @@
         <f>+VLOOKUP($C68,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -12023,7 +12148,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -12042,8 +12167,11 @@
         <f>+VLOOKUP($C70,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -12063,7 +12191,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -12083,7 +12211,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -12103,7 +12231,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -12122,8 +12250,11 @@
         <f>+VLOOKUP($C74,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -12143,7 +12274,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -12162,8 +12293,11 @@
         <f>+VLOOKUP($C76,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -12183,7 +12317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -12203,7 +12337,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -12223,7 +12357,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -12243,7 +12377,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -12263,7 +12397,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -12283,7 +12417,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -12302,8 +12436,11 @@
         <f>+VLOOKUP($C83,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -12322,8 +12459,11 @@
         <f>+VLOOKUP($C84,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -12342,8 +12482,11 @@
         <f>+VLOOKUP($C85,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -12363,7 +12506,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -12383,7 +12526,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -12402,8 +12545,11 @@
         <f>+VLOOKUP($C88,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -12422,8 +12568,11 @@
         <f>+VLOOKUP($C89,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -12442,8 +12591,11 @@
         <f>+VLOOKUP($C90,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -12462,8 +12614,11 @@
         <f>+VLOOKUP($C91,'[1]7020 Pkg Data'!$A$1:$C$398,2,FALSE)</f>
         <v>35</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -12483,7 +12638,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -12503,7 +12658,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -12523,7 +12678,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -12543,7 +12698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>95</v>
       </c>

</xml_diff>